<commit_message>
cpu finished and pass 31 instructions
</commit_message>
<xml_diff>
--- a/cpu信号.xlsx
+++ b/cpu信号.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\86152\Desktop\cpu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7DCB908-3B79-4694-B049-649D5ECE85E7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F265ACC3-3B4E-4A1D-9059-E73C3EDBC437}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9012" xr2:uid="{C2DC2732-0BFD-45BD-A133-A32E9AD8858D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="71">
   <si>
     <t>PCReg_ena</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -106,10 +106,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>EXT1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>EXT5</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -298,15 +294,11 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>MUX8</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>0</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1</t>
+    <t>IM[20:16]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>01</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -870,22 +862,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76CF5A8A-983D-4B29-808B-ABCF8F324274}">
-  <dimension ref="A1:HI32"/>
+  <dimension ref="A1:HG32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R31" sqref="R31"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="11" max="16" width="6.77734375" style="20" customWidth="1"/>
-    <col min="17" max="18" width="9.77734375" style="21" customWidth="1"/>
-    <col min="19" max="19" width="8.88671875" style="20"/>
-    <col min="24" max="27" width="6.77734375" customWidth="1"/>
+    <col min="17" max="17" width="9.77734375" style="21" customWidth="1"/>
+    <col min="18" max="18" width="8.88671875" style="20"/>
+    <col min="23" max="25" width="6.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:217" ht="23.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:215" ht="23.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -933,39 +925,35 @@
         <v>14</v>
       </c>
       <c r="Q1" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="R1" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="S1" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="13" t="s">
+      <c r="S1" s="13" t="s">
         <v>16</v>
       </c>
+      <c r="T1" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="U1" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="W1" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="W1" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="X1" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="Y1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="Z1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="AA1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="AB1" s="4"/>
+      <c r="Z1" s="4"/>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
       <c r="AE1" s="1"/>
@@ -1153,39 +1141,37 @@
       <c r="HE1" s="1"/>
       <c r="HF1" s="1"/>
       <c r="HG1" s="1"/>
-      <c r="HH1" s="1"/>
-      <c r="HI1" s="1"/>
     </row>
-    <row r="2" spans="1:217" ht="18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:215" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="6">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0</v>
+      </c>
+      <c r="D2" s="6">
+        <v>0</v>
+      </c>
+      <c r="E2" s="6">
+        <v>0</v>
+      </c>
+      <c r="F2" s="6">
+        <v>1</v>
+      </c>
+      <c r="G2" s="6">
+        <v>1</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="6">
-        <v>1</v>
-      </c>
-      <c r="C2" s="6">
-        <v>0</v>
-      </c>
-      <c r="D2" s="6">
-        <v>0</v>
-      </c>
-      <c r="E2" s="6">
-        <v>0</v>
-      </c>
-      <c r="F2" s="6">
-        <v>1</v>
-      </c>
-      <c r="G2" s="6">
-        <v>1</v>
-      </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>26</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>27</v>
       </c>
       <c r="K2" s="17">
         <v>0</v>
@@ -1202,32 +1188,30 @@
         <v>0</v>
       </c>
       <c r="Q2" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="R2" s="18"/>
-      <c r="S2" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="T2" s="14">
+        <v>27</v>
+      </c>
+      <c r="R2" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="S2" s="14">
+        <v>0</v>
+      </c>
+      <c r="T2" s="7">
         <v>0</v>
       </c>
       <c r="U2" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V2" s="7">
-        <v>1</v>
-      </c>
-      <c r="W2" s="7">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="W2" s="8"/>
       <c r="X2" s="8"/>
       <c r="Y2" s="8"/>
-      <c r="Z2" s="8"/>
-      <c r="AA2" s="8"/>
     </row>
-    <row r="3" spans="1:217" ht="18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:215" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" s="6">
         <v>1</v>
@@ -1248,13 +1232,13 @@
         <v>1</v>
       </c>
       <c r="H3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="J3" s="6" t="s">
         <v>26</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>27</v>
       </c>
       <c r="K3" s="17">
         <v>0</v>
@@ -1271,13 +1255,15 @@
         <v>0</v>
       </c>
       <c r="Q3" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="R3" s="18"/>
-      <c r="S3" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="T3" s="14">
+        <v>27</v>
+      </c>
+      <c r="R3" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="S3" s="14">
+        <v>0</v>
+      </c>
+      <c r="T3" s="7">
         <v>0</v>
       </c>
       <c r="U3" s="7">
@@ -1286,17 +1272,13 @@
       <c r="V3" s="7">
         <v>0</v>
       </c>
-      <c r="W3" s="7">
-        <v>0</v>
-      </c>
+      <c r="W3" s="8"/>
       <c r="X3" s="8"/>
       <c r="Y3" s="8"/>
-      <c r="Z3" s="8"/>
-      <c r="AA3" s="8"/>
     </row>
-    <row r="4" spans="1:217" ht="18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:215" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" s="6">
         <v>1</v>
@@ -1317,13 +1299,13 @@
         <v>1</v>
       </c>
       <c r="H4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="J4" s="6" t="s">
         <v>26</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>27</v>
       </c>
       <c r="K4" s="17">
         <v>0</v>
@@ -1340,32 +1322,30 @@
         <v>0</v>
       </c>
       <c r="Q4" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="R4" s="18"/>
-      <c r="S4" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="T4" s="14">
+        <v>27</v>
+      </c>
+      <c r="R4" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="S4" s="14">
+        <v>0</v>
+      </c>
+      <c r="T4" s="7">
         <v>0</v>
       </c>
       <c r="U4" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V4" s="7">
         <v>1</v>
       </c>
-      <c r="W4" s="7">
-        <v>1</v>
-      </c>
+      <c r="W4" s="8"/>
       <c r="X4" s="8"/>
       <c r="Y4" s="8"/>
-      <c r="Z4" s="8"/>
-      <c r="AA4" s="8"/>
     </row>
-    <row r="5" spans="1:217" ht="18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:215" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="6">
         <v>1</v>
@@ -1386,13 +1366,13 @@
         <v>1</v>
       </c>
       <c r="H5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="J5" s="6" t="s">
         <v>26</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>27</v>
       </c>
       <c r="K5" s="17">
         <v>0</v>
@@ -1409,32 +1389,30 @@
         <v>0</v>
       </c>
       <c r="Q5" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="R5" s="18"/>
-      <c r="S5" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="T5" s="14">
+        <v>27</v>
+      </c>
+      <c r="R5" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="S5" s="14">
+        <v>0</v>
+      </c>
+      <c r="T5" s="7">
         <v>0</v>
       </c>
       <c r="U5" s="7">
         <v>0</v>
       </c>
       <c r="V5" s="7">
-        <v>0</v>
-      </c>
-      <c r="W5" s="7">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="W5" s="8"/>
       <c r="X5" s="8"/>
       <c r="Y5" s="8"/>
-      <c r="Z5" s="8"/>
-      <c r="AA5" s="8"/>
     </row>
-    <row r="6" spans="1:217" ht="18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:215" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="6">
         <v>1</v>
@@ -1455,13 +1433,13 @@
         <v>1</v>
       </c>
       <c r="H6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="J6" s="6" t="s">
         <v>26</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>27</v>
       </c>
       <c r="K6" s="17">
         <v>0</v>
@@ -1478,59 +1456,57 @@
         <v>0</v>
       </c>
       <c r="Q6" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="R6" s="18"/>
-      <c r="S6" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="T6" s="14">
-        <v>0</v>
+        <v>27</v>
+      </c>
+      <c r="R6" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="S6" s="14">
+        <v>0</v>
+      </c>
+      <c r="T6" s="7">
+        <v>1</v>
       </c>
       <c r="U6" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V6" s="7">
         <v>0</v>
       </c>
-      <c r="W6" s="7">
-        <v>0</v>
-      </c>
+      <c r="W6" s="8"/>
       <c r="X6" s="8"/>
       <c r="Y6" s="8"/>
-      <c r="Z6" s="8"/>
-      <c r="AA6" s="8"/>
     </row>
-    <row r="7" spans="1:217" ht="18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:215" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="6">
+        <v>1</v>
+      </c>
+      <c r="C7" s="6">
+        <v>0</v>
+      </c>
+      <c r="D7" s="6">
+        <v>0</v>
+      </c>
+      <c r="E7" s="6">
+        <v>0</v>
+      </c>
+      <c r="F7" s="6">
+        <v>1</v>
+      </c>
+      <c r="G7" s="6">
+        <v>1</v>
+      </c>
+      <c r="H7" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="6">
-        <v>1</v>
-      </c>
-      <c r="C7" s="6">
-        <v>0</v>
-      </c>
-      <c r="D7" s="6">
-        <v>0</v>
-      </c>
-      <c r="E7" s="6">
-        <v>0</v>
-      </c>
-      <c r="F7" s="6">
-        <v>1</v>
-      </c>
-      <c r="G7" s="6">
-        <v>1</v>
-      </c>
-      <c r="H7" s="6" t="s">
+      <c r="I7" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="J7" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>36</v>
       </c>
       <c r="K7" s="17">
         <v>0</v>
@@ -1547,32 +1523,30 @@
         <v>0</v>
       </c>
       <c r="Q7" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="R7" s="18"/>
-      <c r="S7" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="T7" s="14">
-        <v>0</v>
+        <v>27</v>
+      </c>
+      <c r="R7" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="S7" s="14">
+        <v>0</v>
+      </c>
+      <c r="T7" s="7">
+        <v>1</v>
       </c>
       <c r="U7" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V7" s="7">
-        <v>0</v>
-      </c>
-      <c r="W7" s="7">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="W7" s="8"/>
       <c r="X7" s="8"/>
       <c r="Y7" s="8"/>
-      <c r="Z7" s="8"/>
-      <c r="AA7" s="8"/>
     </row>
-    <row r="8" spans="1:217" ht="18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:215" ht="18" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8" s="6">
         <v>1</v>
@@ -1593,13 +1567,13 @@
         <v>1</v>
       </c>
       <c r="H8" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I8" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="J8" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>36</v>
       </c>
       <c r="K8" s="17">
         <v>0</v>
@@ -1616,32 +1590,30 @@
         <v>0</v>
       </c>
       <c r="Q8" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="R8" s="18"/>
-      <c r="S8" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="T8" s="14">
-        <v>0</v>
+        <v>27</v>
+      </c>
+      <c r="R8" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="S8" s="14">
+        <v>0</v>
+      </c>
+      <c r="T8" s="7">
+        <v>1</v>
       </c>
       <c r="U8" s="7">
         <v>1</v>
       </c>
       <c r="V8" s="7">
-        <v>1</v>
-      </c>
-      <c r="W8" s="7">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="W8" s="8"/>
       <c r="X8" s="8"/>
       <c r="Y8" s="8"/>
-      <c r="Z8" s="8"/>
-      <c r="AA8" s="8"/>
     </row>
-    <row r="9" spans="1:217" ht="18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:215" ht="18" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" s="6">
         <v>1</v>
@@ -1662,13 +1634,13 @@
         <v>1</v>
       </c>
       <c r="H9" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I9" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="I9" s="6" t="s">
+      <c r="J9" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>36</v>
       </c>
       <c r="K9" s="17">
         <v>0</v>
@@ -1685,14 +1657,16 @@
         <v>0</v>
       </c>
       <c r="Q9" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="R9" s="18"/>
-      <c r="S9" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="T9" s="14">
-        <v>0</v>
+        <v>27</v>
+      </c>
+      <c r="R9" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="S9" s="14">
+        <v>0</v>
+      </c>
+      <c r="T9" s="7">
+        <v>1</v>
       </c>
       <c r="U9" s="7">
         <v>1</v>
@@ -1700,17 +1674,13 @@
       <c r="V9" s="7">
         <v>1</v>
       </c>
-      <c r="W9" s="7">
-        <v>1</v>
-      </c>
+      <c r="W9" s="8"/>
       <c r="X9" s="8"/>
       <c r="Y9" s="8"/>
-      <c r="Z9" s="8"/>
-      <c r="AA9" s="8"/>
     </row>
-    <row r="10" spans="1:217" ht="18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:215" ht="18" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B10" s="6">
         <v>1</v>
@@ -1731,13 +1701,13 @@
         <v>1</v>
       </c>
       <c r="H10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I10" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="I10" s="6" t="s">
+      <c r="J10" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>36</v>
       </c>
       <c r="K10" s="17">
         <v>0</v>
@@ -1754,36 +1724,30 @@
         <v>0</v>
       </c>
       <c r="Q10" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="R10" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="S10" s="18">
+        <v>27</v>
+      </c>
+      <c r="R10" s="18">
         <v>11</v>
       </c>
-      <c r="T10" s="14">
-        <v>1</v>
+      <c r="S10" s="14">
+        <v>1</v>
+      </c>
+      <c r="T10" s="7">
+        <v>0</v>
       </c>
       <c r="U10" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V10" s="7">
         <v>1</v>
       </c>
-      <c r="W10" s="7">
-        <v>1</v>
-      </c>
-      <c r="X10" s="10"/>
-      <c r="Y10" s="8">
-        <v>0</v>
-      </c>
-      <c r="Z10" s="8"/>
-      <c r="AA10" s="8"/>
+      <c r="W10" s="10"/>
+      <c r="X10" s="8"/>
+      <c r="Y10" s="8"/>
     </row>
-    <row r="11" spans="1:217" ht="18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:215" ht="18" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B11" s="6">
         <v>1</v>
@@ -1804,13 +1768,13 @@
         <v>1</v>
       </c>
       <c r="H11" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I11" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="J11" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>36</v>
       </c>
       <c r="K11" s="17">
         <v>0</v>
@@ -1827,32 +1791,30 @@
         <v>0</v>
       </c>
       <c r="Q11" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="R11" s="18"/>
-      <c r="S11" s="18">
+        <v>27</v>
+      </c>
+      <c r="R11" s="18">
         <v>11</v>
       </c>
-      <c r="T11" s="14">
-        <v>1</v>
+      <c r="S11" s="14">
+        <v>1</v>
+      </c>
+      <c r="T11" s="7">
+        <v>0</v>
       </c>
       <c r="U11" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V11" s="7">
-        <v>1</v>
-      </c>
-      <c r="W11" s="7">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="W11" s="8"/>
       <c r="X11" s="8"/>
       <c r="Y11" s="8"/>
-      <c r="Z11" s="8"/>
-      <c r="AA11" s="8"/>
     </row>
-    <row r="12" spans="1:217" ht="18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:215" ht="18" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B12" s="6">
         <v>1</v>
@@ -1874,10 +1836,10 @@
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J12" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>36</v>
       </c>
       <c r="K12" s="17">
         <v>0</v>
@@ -1896,34 +1858,32 @@
         <v>0</v>
       </c>
       <c r="Q12" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="R12" s="18"/>
-      <c r="S12" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="T12" s="14">
+        <v>27</v>
+      </c>
+      <c r="R12" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="S12" s="14">
+        <v>1</v>
+      </c>
+      <c r="T12" s="7">
         <v>1</v>
       </c>
       <c r="U12" s="7">
         <v>1</v>
       </c>
-      <c r="V12" s="7">
-        <v>1</v>
-      </c>
-      <c r="W12" s="11" t="s">
+      <c r="V12" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="W12" s="8"/>
+      <c r="X12" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="8"/>
+    </row>
+    <row r="13" spans="1:215" ht="18" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
         <v>42</v>
-      </c>
-      <c r="X12" s="8"/>
-      <c r="Y12" s="8"/>
-      <c r="Z12" s="8">
-        <v>0</v>
-      </c>
-      <c r="AA12" s="8"/>
-    </row>
-    <row r="13" spans="1:217" ht="18" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
-        <v>43</v>
       </c>
       <c r="B13" s="6">
         <v>1</v>
@@ -1945,10 +1905,10 @@
       </c>
       <c r="H13" s="6"/>
       <c r="I13" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J13" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>36</v>
       </c>
       <c r="K13" s="17">
         <v>0</v>
@@ -1967,34 +1927,32 @@
         <v>0</v>
       </c>
       <c r="Q13" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="R13" s="18"/>
-      <c r="S13" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="T13" s="14">
+        <v>27</v>
+      </c>
+      <c r="R13" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="S13" s="14">
+        <v>1</v>
+      </c>
+      <c r="T13" s="7">
         <v>1</v>
       </c>
       <c r="U13" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V13" s="7">
-        <v>0</v>
-      </c>
-      <c r="W13" s="7">
-        <v>1</v>
-      </c>
-      <c r="X13" s="8"/>
+        <v>1</v>
+      </c>
+      <c r="W13" s="8"/>
+      <c r="X13" s="8">
+        <v>0</v>
+      </c>
       <c r="Y13" s="8"/>
-      <c r="Z13" s="8">
-        <v>0</v>
-      </c>
-      <c r="AA13" s="8"/>
     </row>
-    <row r="14" spans="1:217" ht="18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:215" ht="18" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B14" s="6">
         <v>1</v>
@@ -2016,10 +1974,10 @@
       </c>
       <c r="H14" s="6"/>
       <c r="I14" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J14" s="6" t="s">
         <v>26</v>
-      </c>
-      <c r="J14" s="6" t="s">
-        <v>27</v>
       </c>
       <c r="K14" s="17">
         <v>0</v>
@@ -2038,34 +1996,32 @@
         <v>0</v>
       </c>
       <c r="Q14" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="R14" s="18"/>
-      <c r="S14" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="T14" s="14">
+        <v>27</v>
+      </c>
+      <c r="R14" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="S14" s="14">
+        <v>1</v>
+      </c>
+      <c r="T14" s="7">
         <v>1</v>
       </c>
       <c r="U14" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V14" s="7">
         <v>0</v>
       </c>
-      <c r="W14" s="7">
-        <v>0</v>
-      </c>
-      <c r="X14" s="8"/>
+      <c r="W14" s="8"/>
+      <c r="X14" s="8">
+        <v>0</v>
+      </c>
       <c r="Y14" s="8"/>
-      <c r="Z14" s="8">
-        <v>0</v>
-      </c>
-      <c r="AA14" s="8"/>
     </row>
-    <row r="15" spans="1:217" ht="18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:215" ht="18" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B15" s="6">
         <v>1</v>
@@ -2086,13 +2042,13 @@
         <v>1</v>
       </c>
       <c r="H15" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I15" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I15" s="6" t="s">
+      <c r="J15" s="6" t="s">
         <v>26</v>
-      </c>
-      <c r="J15" s="6" t="s">
-        <v>27</v>
       </c>
       <c r="K15" s="17">
         <v>0</v>
@@ -2111,34 +2067,32 @@
         <v>0</v>
       </c>
       <c r="Q15" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="R15" s="18"/>
-      <c r="S15" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="T15" s="14">
+        <v>27</v>
+      </c>
+      <c r="R15" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="S15" s="14">
+        <v>1</v>
+      </c>
+      <c r="T15" s="7">
         <v>1</v>
       </c>
       <c r="U15" s="7">
         <v>1</v>
       </c>
-      <c r="V15" s="7">
-        <v>1</v>
-      </c>
-      <c r="W15" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="X15" s="8"/>
+      <c r="V15" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="W15" s="8"/>
+      <c r="X15" s="8">
+        <v>0</v>
+      </c>
       <c r="Y15" s="8"/>
-      <c r="Z15" s="8">
-        <v>0</v>
-      </c>
-      <c r="AA15" s="8"/>
     </row>
-    <row r="16" spans="1:217" ht="18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:215" ht="18" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B16" s="6">
         <v>1</v>
@@ -2159,13 +2113,13 @@
         <v>1</v>
       </c>
       <c r="H16" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I16" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I16" s="6" t="s">
+      <c r="J16" s="6" t="s">
         <v>26</v>
-      </c>
-      <c r="J16" s="6" t="s">
-        <v>27</v>
       </c>
       <c r="K16" s="17">
         <v>0</v>
@@ -2184,34 +2138,32 @@
         <v>0</v>
       </c>
       <c r="Q16" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="R16" s="18"/>
-      <c r="S16" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="T16" s="14">
+        <v>27</v>
+      </c>
+      <c r="R16" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="S16" s="14">
+        <v>1</v>
+      </c>
+      <c r="T16" s="7">
         <v>1</v>
       </c>
       <c r="U16" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V16" s="7">
-        <v>0</v>
-      </c>
-      <c r="W16" s="7">
-        <v>1</v>
-      </c>
-      <c r="X16" s="8"/>
+        <v>1</v>
+      </c>
+      <c r="W16" s="8"/>
+      <c r="X16" s="8">
+        <v>0</v>
+      </c>
       <c r="Y16" s="8"/>
-      <c r="Z16" s="8">
-        <v>0</v>
-      </c>
-      <c r="AA16" s="8"/>
     </row>
-    <row r="17" spans="1:27" ht="18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" ht="18" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B17" s="6">
         <v>1</v>
@@ -2232,13 +2184,13 @@
         <v>1</v>
       </c>
       <c r="H17" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I17" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I17" s="6" t="s">
+      <c r="J17" s="6" t="s">
         <v>26</v>
-      </c>
-      <c r="J17" s="6" t="s">
-        <v>27</v>
       </c>
       <c r="K17" s="17">
         <v>0</v>
@@ -2257,34 +2209,32 @@
         <v>0</v>
       </c>
       <c r="Q17" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="R17" s="18"/>
-      <c r="S17" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="T17" s="14">
+        <v>27</v>
+      </c>
+      <c r="R17" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="S17" s="14">
+        <v>1</v>
+      </c>
+      <c r="T17" s="7">
         <v>1</v>
       </c>
       <c r="U17" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V17" s="7">
         <v>0</v>
       </c>
-      <c r="W17" s="7">
-        <v>0</v>
-      </c>
-      <c r="X17" s="8"/>
+      <c r="W17" s="8"/>
+      <c r="X17" s="8">
+        <v>0</v>
+      </c>
       <c r="Y17" s="8"/>
-      <c r="Z17" s="8">
-        <v>0</v>
-      </c>
-      <c r="AA17" s="8"/>
     </row>
-    <row r="18" spans="1:27" ht="18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" ht="18" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B18" s="6">
         <v>1</v>
@@ -2305,7 +2255,7 @@
         <v>0</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
@@ -2323,19 +2273,17 @@
       <c r="P18" s="17"/>
       <c r="Q18" s="18"/>
       <c r="R18" s="18"/>
-      <c r="S18" s="18"/>
-      <c r="T18" s="14"/>
+      <c r="S18" s="14"/>
+      <c r="T18" s="7"/>
       <c r="U18" s="7"/>
       <c r="V18" s="7"/>
-      <c r="W18" s="7"/>
+      <c r="W18" s="8"/>
       <c r="X18" s="8"/>
       <c r="Y18" s="8"/>
-      <c r="Z18" s="8"/>
-      <c r="AA18" s="8"/>
     </row>
-    <row r="19" spans="1:27" ht="18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" ht="18" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B19" s="6">
         <v>1</v>
@@ -2356,11 +2304,11 @@
         <v>1</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I19" s="6"/>
       <c r="J19" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K19" s="17">
         <v>0</v>
@@ -2377,34 +2325,32 @@
         <v>1</v>
       </c>
       <c r="Q19" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="R19" s="18"/>
-      <c r="S19" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="T19" s="14">
+        <v>55</v>
+      </c>
+      <c r="R19" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="S19" s="14">
+        <v>0</v>
+      </c>
+      <c r="T19" s="7">
         <v>0</v>
       </c>
       <c r="U19" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V19" s="7">
-        <v>1</v>
-      </c>
-      <c r="W19" s="7">
-        <v>0</v>
-      </c>
-      <c r="X19" s="8">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="W19" s="8">
+        <v>1</v>
+      </c>
+      <c r="X19" s="8"/>
       <c r="Y19" s="8"/>
-      <c r="Z19" s="8"/>
-      <c r="AA19" s="8"/>
     </row>
-    <row r="20" spans="1:27" ht="18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" ht="18" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B20" s="6">
         <v>1</v>
@@ -2425,11 +2371,11 @@
         <v>1</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I20" s="6"/>
       <c r="J20" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K20" s="17">
         <v>0</v>
@@ -2446,13 +2392,15 @@
         <v>1</v>
       </c>
       <c r="Q20" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="R20" s="18"/>
-      <c r="S20" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="T20" s="14">
+        <v>55</v>
+      </c>
+      <c r="R20" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="S20" s="14">
+        <v>0</v>
+      </c>
+      <c r="T20" s="7">
         <v>0</v>
       </c>
       <c r="U20" s="7">
@@ -2461,19 +2409,15 @@
       <c r="V20" s="7">
         <v>0</v>
       </c>
-      <c r="W20" s="7">
-        <v>0</v>
-      </c>
-      <c r="X20" s="8">
-        <v>1</v>
-      </c>
+      <c r="W20" s="8">
+        <v>1</v>
+      </c>
+      <c r="X20" s="8"/>
       <c r="Y20" s="8"/>
-      <c r="Z20" s="8"/>
-      <c r="AA20" s="8"/>
     </row>
-    <row r="21" spans="1:27" ht="18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" ht="18" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B21" s="6">
         <v>1</v>
@@ -2494,11 +2438,11 @@
         <v>1</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I21" s="6"/>
       <c r="J21" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K21" s="17">
         <v>0</v>
@@ -2515,34 +2459,32 @@
         <v>1</v>
       </c>
       <c r="Q21" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="R21" s="18"/>
-      <c r="S21" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="T21" s="14">
-        <v>0</v>
+        <v>55</v>
+      </c>
+      <c r="R21" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="S21" s="14">
+        <v>0</v>
+      </c>
+      <c r="T21" s="7">
+        <v>1</v>
       </c>
       <c r="U21" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V21" s="7">
         <v>0</v>
       </c>
-      <c r="W21" s="7">
-        <v>0</v>
-      </c>
-      <c r="X21" s="8">
-        <v>0</v>
-      </c>
+      <c r="W21" s="8">
+        <v>0</v>
+      </c>
+      <c r="X21" s="8"/>
       <c r="Y21" s="8"/>
-      <c r="Z21" s="8"/>
-      <c r="AA21" s="8"/>
     </row>
-    <row r="22" spans="1:27" ht="18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B22" s="6">
         <v>1</v>
@@ -2563,11 +2505,11 @@
         <v>1</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I22" s="6"/>
       <c r="J22" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K22" s="17">
         <v>0</v>
@@ -2584,34 +2526,32 @@
         <v>1</v>
       </c>
       <c r="Q22" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="R22" s="18"/>
-      <c r="S22" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="T22" s="14">
-        <v>0</v>
+        <v>55</v>
+      </c>
+      <c r="R22" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="S22" s="14">
+        <v>0</v>
+      </c>
+      <c r="T22" s="7">
+        <v>1</v>
       </c>
       <c r="U22" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V22" s="7">
-        <v>0</v>
-      </c>
-      <c r="W22" s="7">
-        <v>1</v>
-      </c>
-      <c r="X22" s="8">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="W22" s="8">
+        <v>0</v>
+      </c>
+      <c r="X22" s="8"/>
       <c r="Y22" s="8"/>
-      <c r="Z22" s="8"/>
-      <c r="AA22" s="8"/>
     </row>
-    <row r="23" spans="1:27" ht="18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" ht="18" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B23" s="6">
         <v>1</v>
@@ -2632,11 +2572,11 @@
         <v>1</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I23" s="6"/>
       <c r="J23" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K23" s="17">
         <v>0</v>
@@ -2653,35 +2593,33 @@
         <v>1</v>
       </c>
       <c r="Q23" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="R23" s="18"/>
-      <c r="S23" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="R23" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="S23" s="14">
+        <v>0</v>
+      </c>
+      <c r="T23" s="7">
+        <v>1</v>
+      </c>
+      <c r="U23" s="7">
+        <v>1</v>
+      </c>
+      <c r="V23" s="7">
+        <v>0</v>
+      </c>
+      <c r="W23" s="8">
+        <v>0</v>
+      </c>
+      <c r="X23" s="8"/>
+      <c r="Y23" s="8"/>
+    </row>
+    <row r="24" spans="1:25" ht="18" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="T23" s="14">
-        <v>0</v>
-      </c>
-      <c r="U23" s="7">
-        <v>1</v>
-      </c>
-      <c r="V23" s="7">
-        <v>1</v>
-      </c>
-      <c r="W23" s="7">
-        <v>0</v>
-      </c>
-      <c r="X23" s="8">
-        <v>0</v>
-      </c>
-      <c r="Y23" s="8"/>
-      <c r="Z23" s="8"/>
-      <c r="AA23" s="8"/>
-    </row>
-    <row r="24" spans="1:27" ht="18" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
-        <v>55</v>
-      </c>
       <c r="B24" s="6">
         <v>1</v>
       </c>
@@ -2701,10 +2639,12 @@
         <v>1</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
+      <c r="J24" s="6" t="s">
+        <v>69</v>
+      </c>
       <c r="K24" s="17">
         <v>0</v>
       </c>
@@ -2719,34 +2659,34 @@
       <c r="P24" s="17">
         <v>1</v>
       </c>
-      <c r="Q24" s="18"/>
-      <c r="R24" s="18"/>
-      <c r="S24" s="18" t="s">
+      <c r="Q24" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="R24" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="S24" s="14">
+        <v>0</v>
+      </c>
+      <c r="T24" s="7">
+        <v>0</v>
+      </c>
+      <c r="U24" s="7">
+        <v>0</v>
+      </c>
+      <c r="V24" s="7">
+        <v>0</v>
+      </c>
+      <c r="W24" s="8">
+        <v>1</v>
+      </c>
+      <c r="X24" s="8"/>
+      <c r="Y24" s="8"/>
+    </row>
+    <row r="25" spans="1:25" ht="18" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="T24" s="14">
-        <v>0</v>
-      </c>
-      <c r="U24" s="7">
-        <v>0</v>
-      </c>
-      <c r="V24" s="7">
-        <v>1</v>
-      </c>
-      <c r="W24" s="7">
-        <v>0</v>
-      </c>
-      <c r="X24" s="8">
-        <v>1</v>
-      </c>
-      <c r="Y24" s="8"/>
-      <c r="Z24" s="8"/>
-      <c r="AA24" s="8"/>
-    </row>
-    <row r="25" spans="1:27" ht="18" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
-        <v>57</v>
-      </c>
       <c r="B25" s="6">
         <v>1</v>
       </c>
@@ -2766,10 +2706,10 @@
         <v>0</v>
       </c>
       <c r="H25" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I25" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="I25" s="6" t="s">
-        <v>26</v>
       </c>
       <c r="J25" s="6"/>
       <c r="K25" s="17">
@@ -2788,29 +2728,27 @@
       </c>
       <c r="Q25" s="18"/>
       <c r="R25" s="18"/>
-      <c r="S25" s="18"/>
-      <c r="T25" s="14">
+      <c r="S25" s="14">
+        <v>0</v>
+      </c>
+      <c r="T25" s="7">
         <v>0</v>
       </c>
       <c r="U25" s="7">
         <v>0</v>
       </c>
       <c r="V25" s="7">
-        <v>1</v>
-      </c>
-      <c r="W25" s="7">
-        <v>0</v>
-      </c>
-      <c r="X25" s="8">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="W25" s="8">
+        <v>1</v>
+      </c>
+      <c r="X25" s="8"/>
       <c r="Y25" s="8"/>
-      <c r="Z25" s="8"/>
-      <c r="AA25" s="8"/>
     </row>
-    <row r="26" spans="1:27" ht="18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" ht="18" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B26" s="6">
         <v>1</v>
@@ -2831,17 +2769,17 @@
         <v>0</v>
       </c>
       <c r="H26" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I26" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="I26" s="6" t="s">
-        <v>26</v>
       </c>
       <c r="J26" s="6"/>
       <c r="K26" s="17">
         <v>0</v>
       </c>
       <c r="L26" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M26" s="17"/>
       <c r="N26" s="17">
@@ -2855,29 +2793,27 @@
       </c>
       <c r="Q26" s="18"/>
       <c r="R26" s="18"/>
-      <c r="S26" s="18"/>
-      <c r="T26" s="14">
+      <c r="S26" s="14">
+        <v>0</v>
+      </c>
+      <c r="T26" s="7">
         <v>0</v>
       </c>
       <c r="U26" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V26" s="7">
         <v>1</v>
       </c>
-      <c r="W26" s="7">
-        <v>1</v>
-      </c>
+      <c r="W26" s="8"/>
       <c r="X26" s="8"/>
-      <c r="Y26" s="8"/>
-      <c r="Z26" s="8"/>
-      <c r="AA26" s="8">
+      <c r="Y26" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:27" ht="18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" ht="18" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B27" s="6">
         <v>1</v>
@@ -2898,17 +2834,17 @@
         <v>0</v>
       </c>
       <c r="H27" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I27" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="I27" s="6" t="s">
-        <v>26</v>
       </c>
       <c r="J27" s="6"/>
       <c r="K27" s="17">
         <v>0</v>
       </c>
       <c r="L27" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M27" s="17"/>
       <c r="N27" s="17">
@@ -2922,29 +2858,27 @@
       </c>
       <c r="Q27" s="18"/>
       <c r="R27" s="18"/>
-      <c r="S27" s="18"/>
-      <c r="T27" s="14">
+      <c r="S27" s="14">
+        <v>0</v>
+      </c>
+      <c r="T27" s="7">
         <v>0</v>
       </c>
       <c r="U27" s="7">
         <v>0</v>
       </c>
       <c r="V27" s="7">
-        <v>0</v>
-      </c>
-      <c r="W27" s="7">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="W27" s="8"/>
       <c r="X27" s="8"/>
-      <c r="Y27" s="8"/>
-      <c r="Z27" s="8"/>
-      <c r="AA27" s="8">
+      <c r="Y27" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:27" ht="18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25" ht="18" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B28" s="6">
         <v>1</v>
@@ -2965,11 +2899,11 @@
         <v>1</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I28" s="6"/>
       <c r="J28" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K28" s="17">
         <v>0</v>
@@ -2986,38 +2920,32 @@
         <v>1</v>
       </c>
       <c r="Q28" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="R28" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="S28" s="19">
+        <v>55</v>
+      </c>
+      <c r="R28" s="19">
         <v>11</v>
       </c>
-      <c r="T28" s="14">
-        <v>1</v>
+      <c r="S28" s="14">
+        <v>1</v>
+      </c>
+      <c r="T28" s="7">
+        <v>0</v>
       </c>
       <c r="U28" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V28" s="7">
         <v>1</v>
       </c>
-      <c r="W28" s="7">
-        <v>1</v>
-      </c>
-      <c r="X28" s="8">
-        <v>1</v>
-      </c>
-      <c r="Y28" s="8">
-        <v>0</v>
-      </c>
-      <c r="Z28" s="8"/>
-      <c r="AA28" s="8"/>
+      <c r="W28" s="8">
+        <v>1</v>
+      </c>
+      <c r="X28" s="8"/>
+      <c r="Y28" s="8"/>
     </row>
-    <row r="29" spans="1:27" ht="18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" ht="18" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B29" s="6">
         <v>1</v>
@@ -3038,11 +2966,11 @@
         <v>1</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I29" s="6"/>
       <c r="J29" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K29" s="17">
         <v>0</v>
@@ -3059,38 +2987,32 @@
         <v>1</v>
       </c>
       <c r="Q29" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="R29" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="S29" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="S29" s="14">
+        <v>1</v>
+      </c>
+      <c r="T29" s="7">
+        <v>0</v>
+      </c>
+      <c r="U29" s="7">
+        <v>1</v>
+      </c>
+      <c r="V29" s="7">
+        <v>0</v>
+      </c>
+      <c r="W29" s="8">
+        <v>1</v>
+      </c>
+      <c r="X29" s="8"/>
+      <c r="Y29" s="8"/>
+    </row>
+    <row r="30" spans="1:25" ht="18" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
         <v>63</v>
-      </c>
-      <c r="T29" s="14">
-        <v>1</v>
-      </c>
-      <c r="U29" s="7">
-        <v>0</v>
-      </c>
-      <c r="V29" s="7">
-        <v>1</v>
-      </c>
-      <c r="W29" s="7">
-        <v>0</v>
-      </c>
-      <c r="X29" s="8">
-        <v>1</v>
-      </c>
-      <c r="Y29" s="8">
-        <v>0</v>
-      </c>
-      <c r="Z29" s="8"/>
-      <c r="AA29" s="8"/>
-    </row>
-    <row r="30" spans="1:27" ht="18" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
-        <v>64</v>
       </c>
       <c r="B30" s="6">
         <v>1</v>
@@ -3113,7 +3035,7 @@
       <c r="H30" s="6"/>
       <c r="I30" s="6"/>
       <c r="J30" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K30" s="17">
         <v>0</v>
@@ -3124,36 +3046,36 @@
       <c r="M30" s="17"/>
       <c r="N30" s="17"/>
       <c r="O30" s="17"/>
-      <c r="P30" s="17"/>
+      <c r="P30" s="17">
+        <v>1</v>
+      </c>
       <c r="Q30" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="R30" s="18"/>
-      <c r="S30" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="T30" s="14">
-        <v>1</v>
+        <v>55</v>
+      </c>
+      <c r="R30" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="S30" s="14">
+        <v>1</v>
+      </c>
+      <c r="T30" s="7">
+        <v>0</v>
       </c>
       <c r="U30" s="7">
         <v>0</v>
       </c>
-      <c r="V30" s="7">
-        <v>0</v>
-      </c>
-      <c r="W30" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="X30" s="8">
-        <v>0</v>
-      </c>
+      <c r="V30" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="W30" s="8">
+        <v>0</v>
+      </c>
+      <c r="X30" s="8"/>
       <c r="Y30" s="8"/>
-      <c r="Z30" s="8"/>
-      <c r="AA30" s="8"/>
     </row>
-    <row r="31" spans="1:27" ht="18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:25" ht="18" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B31" s="6">
         <v>1</v>
@@ -3188,19 +3110,17 @@
       <c r="P31" s="17"/>
       <c r="Q31" s="18"/>
       <c r="R31" s="18"/>
-      <c r="S31" s="18"/>
-      <c r="T31" s="14"/>
+      <c r="S31" s="14"/>
+      <c r="T31" s="7"/>
       <c r="U31" s="7"/>
       <c r="V31" s="7"/>
-      <c r="W31" s="7"/>
+      <c r="W31" s="8"/>
       <c r="X31" s="8"/>
       <c r="Y31" s="8"/>
-      <c r="Z31" s="8"/>
-      <c r="AA31" s="8"/>
     </row>
-    <row r="32" spans="1:27" ht="18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:25" ht="18" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B32" s="6">
         <v>1</v>
@@ -3223,7 +3143,7 @@
       <c r="H32" s="6"/>
       <c r="I32" s="6"/>
       <c r="J32" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K32" s="17">
         <v>1</v>
@@ -3236,23 +3156,22 @@
       <c r="O32" s="17"/>
       <c r="P32" s="17"/>
       <c r="Q32" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="R32" s="18"/>
-      <c r="S32" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="T32" s="14"/>
+        <v>67</v>
+      </c>
+      <c r="R32" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="S32" s="14"/>
+      <c r="T32" s="7"/>
       <c r="U32" s="7"/>
       <c r="V32" s="7"/>
-      <c r="W32" s="7"/>
+      <c r="W32" s="8"/>
       <c r="X32" s="8"/>
       <c r="Y32" s="8"/>
-      <c r="Z32" s="8"/>
-      <c r="AA32" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>